<commit_message>
Update results of test case 20160331 - 001 -> 003
</commit_message>
<xml_diff>
--- a/20160331 - 001/running_logs/logs.xlsx
+++ b/20160331 - 001/running_logs/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
   <si>
     <t>Time</t>
   </si>
@@ -71,6 +71,27 @@
   </si>
   <si>
     <t>20160401_013708</t>
+  </si>
+  <si>
+    <t>20160401_015215</t>
+  </si>
+  <si>
+    <t>convert unicode to ascii, trim "space" and ",", remove multiple spaces, convert to lower</t>
+  </si>
+  <si>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 300</t>
+  </si>
+  <si>
+    <t>20160401_015918</t>
+  </si>
+  <si>
+    <t>20160401_020918</t>
+  </si>
+  <si>
+    <t>20160401_021836</t>
+  </si>
+  <si>
+    <t>20160401_022803</t>
   </si>
 </sst>
 </file>
@@ -402,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -597,6 +618,166 @@
         <v>0.285714285714286</v>
       </c>
     </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>423.191</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7">
+        <v>0.958666666666667</v>
+      </c>
+      <c r="H7">
+        <v>0.996699669966997</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7">
+        <v>0.255102040816327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>600.244</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8">
+        <v>0.963333333333333</v>
+      </c>
+      <c r="H8">
+        <v>0.996699669966997</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>0.224489795918367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>557.882</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9">
+        <v>0.962</v>
+      </c>
+      <c r="H9">
+        <v>0.996699669966997</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9">
+        <v>0.275510204081633</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>567.123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10">
+        <v>0.953333333333333</v>
+      </c>
+      <c r="H10">
+        <v>0.996699669966997</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10">
+        <v>0.23469387755102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>769.718</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11">
+        <v>0.966</v>
+      </c>
+      <c r="H11">
+        <v>0.996699669966997</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11">
+        <v>0.244897959183673</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update test case 20160331 - 001
</commit_message>
<xml_diff>
--- a/20160331 - 001/running_logs/logs.xlsx
+++ b/20160331 - 001/running_logs/logs.xlsx
@@ -43,13 +43,13 @@
     <t>Template Filter</t>
   </si>
   <si>
-    <t>20160401_013003</t>
-  </si>
-  <si>
-    <t>trim "space" and ",", convert unicode to ascii, convert to lower, remove multiple spaces</t>
-  </si>
-  <si>
-    <t>3 features: #ascii/(#ascii+#digit+#punctuation), %kwPhone, #max_digit_skip_0_1</t>
+    <t>20160403_220347</t>
+  </si>
+  <si>
+    <t>convert unicode to ascii, convert to lower, trim "space" and ",", remove multiple spaces</t>
+  </si>
+  <si>
+    <t>4 features: #ascii/(#ascii+#digit+#punctuation), %kwAddress, %kwPhone, #max_digit_skip_0_1</t>
   </si>
   <si>
     <t>Neuron Network</t>
@@ -61,37 +61,37 @@
     <t xml:space="preserve">0 filters: </t>
   </si>
   <si>
-    <t>20160401_013140</t>
-  </si>
-  <si>
-    <t>20160401_013324</t>
-  </si>
-  <si>
-    <t>20160401_013518</t>
-  </si>
-  <si>
-    <t>20160401_013708</t>
-  </si>
-  <si>
-    <t>20160401_015215</t>
-  </si>
-  <si>
-    <t>convert unicode to ascii, trim "space" and ",", remove multiple spaces, convert to lower</t>
+    <t>20160403_220619</t>
+  </si>
+  <si>
+    <t>20160403_225031</t>
+  </si>
+  <si>
+    <t>20160403_225410</t>
+  </si>
+  <si>
+    <t>20160403_225709</t>
+  </si>
+  <si>
+    <t>20160404_024810</t>
+  </si>
+  <si>
+    <t>trim "space" and ",", convert to lower, remove multiple spaces, convert unicode to ascii</t>
   </si>
   <si>
     <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 300</t>
   </si>
   <si>
-    <t>20160401_015918</t>
-  </si>
-  <si>
-    <t>20160401_020918</t>
-  </si>
-  <si>
-    <t>20160401_021836</t>
-  </si>
-  <si>
-    <t>20160401_022803</t>
+    <t>20160404_025448</t>
+  </si>
+  <si>
+    <t>20160404_030648</t>
+  </si>
+  <si>
+    <t>20160404_032232</t>
+  </si>
+  <si>
+    <t>20160404_033731</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>96.662</v>
+        <v>152.133</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -478,7 +478,7 @@
         <v>13</v>
       </c>
       <c r="G2">
-        <v>0.958</v>
+        <v>0.967333333333333</v>
       </c>
       <c r="H2">
         <v>0.996699669966997</v>
@@ -487,7 +487,7 @@
         <v>14</v>
       </c>
       <c r="J2">
-        <v>0.295918367346939</v>
+        <v>0.122448979591837</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -495,7 +495,7 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>104.134</v>
+        <v>2651.614</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -519,7 +519,7 @@
         <v>14</v>
       </c>
       <c r="J3">
-        <v>0.26530612244898</v>
+        <v>0.122448979591837</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -527,7 +527,7 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>113.345</v>
+        <v>219.519</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -542,7 +542,7 @@
         <v>13</v>
       </c>
       <c r="G4">
-        <v>0.952666666666667</v>
+        <v>0.966666666666667</v>
       </c>
       <c r="H4">
         <v>0.996699669966997</v>
@@ -551,7 +551,7 @@
         <v>14</v>
       </c>
       <c r="J4">
-        <v>0.275510204081633</v>
+        <v>0.122448979591837</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -559,7 +559,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>110.835</v>
+        <v>179.266</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -574,7 +574,7 @@
         <v>13</v>
       </c>
       <c r="G5">
-        <v>0.96</v>
+        <v>0.958</v>
       </c>
       <c r="H5">
         <v>0.996699669966997</v>
@@ -583,7 +583,7 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <v>0.275510204081633</v>
+        <v>0.122448979591837</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -591,7 +591,7 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>111.325</v>
+        <v>171.497</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -606,7 +606,7 @@
         <v>13</v>
       </c>
       <c r="G6">
-        <v>0.947333333333333</v>
+        <v>0.957333333333333</v>
       </c>
       <c r="H6">
         <v>0.996699669966997</v>
@@ -615,7 +615,7 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <v>0.285714285714286</v>
+        <v>0.122448979591837</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -623,7 +623,7 @@
         <v>19</v>
       </c>
       <c r="B7">
-        <v>423.191</v>
+        <v>398.191</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -638,7 +638,7 @@
         <v>21</v>
       </c>
       <c r="G7">
-        <v>0.958666666666667</v>
+        <v>0.962</v>
       </c>
       <c r="H7">
         <v>0.996699669966997</v>
@@ -647,7 +647,7 @@
         <v>14</v>
       </c>
       <c r="J7">
-        <v>0.255102040816327</v>
+        <v>0.13265306122449</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -655,7 +655,7 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>600.244</v>
+        <v>719.814</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -670,7 +670,7 @@
         <v>21</v>
       </c>
       <c r="G8">
-        <v>0.963333333333333</v>
+        <v>0.966666666666667</v>
       </c>
       <c r="H8">
         <v>0.996699669966997</v>
@@ -679,7 +679,7 @@
         <v>14</v>
       </c>
       <c r="J8">
-        <v>0.224489795918367</v>
+        <v>0.13265306122449</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -687,7 +687,7 @@
         <v>23</v>
       </c>
       <c r="B9">
-        <v>557.882</v>
+        <v>943.872</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -702,7 +702,7 @@
         <v>21</v>
       </c>
       <c r="G9">
-        <v>0.962</v>
+        <v>0.974</v>
       </c>
       <c r="H9">
         <v>0.996699669966997</v>
@@ -711,7 +711,7 @@
         <v>14</v>
       </c>
       <c r="J9">
-        <v>0.275510204081633</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -719,7 +719,7 @@
         <v>24</v>
       </c>
       <c r="B10">
-        <v>567.123</v>
+        <v>899.649</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -734,7 +734,7 @@
         <v>21</v>
       </c>
       <c r="G10">
-        <v>0.953333333333333</v>
+        <v>0.971333333333333</v>
       </c>
       <c r="H10">
         <v>0.996699669966997</v>
@@ -743,7 +743,7 @@
         <v>14</v>
       </c>
       <c r="J10">
-        <v>0.23469387755102</v>
+        <v>0.13265306122449</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -751,7 +751,7 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <v>769.718</v>
+        <v>560.731</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -766,7 +766,7 @@
         <v>21</v>
       </c>
       <c r="G11">
-        <v>0.966</v>
+        <v>0.972666666666667</v>
       </c>
       <c r="H11">
         <v>0.996699669966997</v>
@@ -775,7 +775,7 @@
         <v>14</v>
       </c>
       <c r="J11">
-        <v>0.244897959183673</v>
+        <v>0.13265306122449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>